<commit_message>
1. Document: Update art work plan in tab 'Sprint Game' & 'Sprint UI'; 2. Project settings : IOS launch settings changed support 64 bit system; 3. GameArena changed: (1) Hero follows geek logic; (2) Bug fixed: Floor enemy in sky; (3) Enemy add 'die' state; (4) Add font HoboStd; (5) First UI hit meter performance changed;
TODO:
Clouds loop logic
</commit_message>
<xml_diff>
--- a/Document/ArtList.xlsx
+++ b/Document/ArtList.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity5_projects\PrimitiveBall\Document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="28035" windowHeight="12105"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="28035" windowHeight="12105" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Total" sheetId="2" r:id="rId1"/>
+    <sheet name="Sprits Game" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprints UI" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>站姿</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -230,6 +236,78 @@
   </si>
   <si>
     <t>英雄大招6个</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprint</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In game content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄大招2个（4月20日更新）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄大招2个（4月27日更新）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英雄大招2个（5月4日更新）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌人（3个，每个敌人 5 个姿势，每个姿势是小动画10帧内，飘在天上的动作）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10个NPC（每个NPC都有一个飞行或行走的动作6帧内）NPC 设定（4月6日更新）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>游戏内：任务条，发射标尺，大招按钮，金币，（高度，距离，速度）HUD，打击次数标示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能加点界面，英雄更换界面，装备界面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁匠铺/商店（购买装备，打造装备，强化装备）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战报UI，大地图设计（按钮编排，界面内容概念图，HUD）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日任务，首页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI调整优化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI指导风格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个风格灵感主要来源于岩壁绘画  用了岩壁材质和涂料涂抹的感觉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字体：HoboStd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -276,7 +354,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -288,6 +366,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -305,12 +389,75 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7219950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>4067175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2" descr="G:\QQdownload\1265342645\Image\C2C\XGL71V(2KJTX~ELOI%FNUMF.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2676525" y="5915025"/>
+          <a:ext cx="7219950" cy="4067175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -352,7 +499,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -387,7 +534,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -643,7 +790,7 @@
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -655,7 +802,7 @@
       <c r="D7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
@@ -665,7 +812,7 @@
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
@@ -675,7 +822,7 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
@@ -685,13 +832,13 @@
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
@@ -821,7 +968,7 @@
       <c r="D31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -834,7 +981,7 @@
       <c r="D32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
@@ -845,7 +992,7 @@
       <c r="D33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
@@ -856,7 +1003,7 @@
       <c r="D34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
@@ -867,7 +1014,7 @@
       <c r="D35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B36" s="2">
@@ -887,104 +1034,104 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A54" s="3" t="s">
@@ -1015,13 +1162,188 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="34.5" customWidth="1"/>
+    <col min="2" max="2" width="76.75" customWidth="1"/>
+    <col min="3" max="3" width="38.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5">
+        <v>42099</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>42106</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>42113</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="65.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>42120</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <v>42127</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <v>42139</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B9" s="3"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="35.125" customWidth="1"/>
+    <col min="2" max="2" width="106.375" customWidth="1"/>
+    <col min="3" max="3" width="69.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="5">
+        <v>42099</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>42106</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>42113</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="81.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>42120</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <v>42127</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <v>42139</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" ht="327" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>